<commit_message>
Cập nhật kết quả test ANN với từng Activation Function khác nhau và Tanh cho kết quả tốt nhất
</commit_message>
<xml_diff>
--- a/Document/TestResultANN.xlsx
+++ b/Document/TestResultANN.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="10455" windowHeight="4620"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="10455" windowHeight="4620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SigmoidTest" sheetId="1" r:id="rId1"/>
+    <sheet name="CompairActivationFunctioin" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="19">
   <si>
     <t>Uptrend</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Accurancy</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>Logarithm</t>
+  </si>
+  <si>
+    <t>Tanh</t>
+  </si>
+  <si>
+    <t>Sine</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -73,12 +88,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,16 +120,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,7 +454,7 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.745</v>
       </c>
       <c r="F2" t="s">
@@ -437,31 +466,31 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.64</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +603,7 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.39500000000000002</v>
       </c>
       <c r="F9" t="s">
@@ -586,31 +615,31 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>0.36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +752,7 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>0.59</v>
       </c>
       <c r="F16" t="s">
@@ -735,31 +764,31 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>0.48</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="2"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +901,7 @@
       <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>0.74</v>
       </c>
       <c r="F23" t="s">
@@ -884,31 +913,31 @@
       <c r="H23" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>0.74</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="2"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1050,7 @@
       <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>0.78500000000000003</v>
       </c>
       <c r="F30" t="s">
@@ -1033,31 +1062,31 @@
       <c r="H30" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>0.495</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="2"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1170,7 +1199,7 @@
       <c r="C37" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>0.60499999999999998</v>
       </c>
       <c r="F37" t="s">
@@ -1182,31 +1211,31 @@
       <c r="H37" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="2">
         <v>0.39500000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="2"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="6"/>
       <c r="G39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1343,12 +1372,300 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.745</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <f>AVERAGE(B2:B7)</f>
+        <v>0.64333333333333331</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:E8" si="0">AVERAGE(C2:C7)</f>
+        <v>0.48333333333333339</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.67666666666666675</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34416666666666668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.495</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.435</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <f>AVERAGE(B12:B17)</f>
+        <v>0.51833333333333331</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:E18" si="1">AVERAGE(C12:C17)</f>
+        <v>0.40416666666666673</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.54416666666666669</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.3175</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>